<commit_message>
modified the Excel recording function so that it overwrites new data every time it is launched
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,82 +441,47 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Код (1,3)</t>
+          <t>Код (3,1)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Код (1,4)</t>
+          <t>Код (4,1)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Код (2,4)</t>
+          <t>Код (4,2)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Код (1,5)</t>
+          <t>Код (5,1)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Код (2,5)</t>
+          <t>Код (5,2)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Код (3,5)</t>
+          <t>Код (5,3)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Код (1,6)</t>
+          <t>Код (6,1)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Код (2,6)</t>
+          <t>Код (6,2)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Код (3,6)</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Код (3,1)</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Код (4,1)</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Код (4,2)</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Код (5,1)</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Код (5,2)</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Код (5,3)</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Код (6,1)</t>
+          <t>Код (6,3)</t>
         </is>
       </c>
     </row>
@@ -537,53 +502,32 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>19</v>
+      </c>
+      <c r="C3" t="n">
         <v>20</v>
-      </c>
-      <c r="C3" t="n">
-        <v>21</v>
       </c>
       <c r="D3" t="n">
         <v>4</v>
       </c>
       <c r="E3" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
         <v>78</v>
       </c>
       <c r="I3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" t="n">
         <v>4</v>
       </c>
-      <c r="K3" t="n">
-        <v>23</v>
-      </c>
-      <c r="L3" t="n">
-        <v>20</v>
-      </c>
-      <c r="M3" t="n">
-        <v>3</v>
-      </c>
-      <c r="N3" t="n">
-        <v>42</v>
-      </c>
-      <c r="O3" t="n">
-        <v>5</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>78</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -595,46 +539,28 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>72</v>
       </c>
       <c r="I4" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J4" t="n">
-        <v>8</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>7</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>36</v>
-      </c>
-      <c r="O4" t="n">
-        <v>7</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>70</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -644,34 +570,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="n">
-        <v>16</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -684,22 +598,16 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I6" t="n">
-        <v>4</v>
-      </c>
-      <c r="L6" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -709,25 +617,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -740,19 +642,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H8" t="n">
-        <v>18</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -762,16 +658,13 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>8</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -781,13 +674,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -796,11 +689,11 @@
           <t>max+9</t>
         </is>
       </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
       <c r="H11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -809,11 +702,11 @@
           <t>max+10</t>
         </is>
       </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
       <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -823,7 +716,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -843,7 +736,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -873,6 +766,26 @@
         </is>
       </c>
       <c r="H18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>max+17</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>max+18</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>